<commit_message>
mask table row reading feature
</commit_message>
<xml_diff>
--- a/data/Audiometry.xlsx
+++ b/data/Audiometry.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasanth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python_workspace\Audiometry-xls-converterv2\Audiometry-xls-converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D736D1-AA1C-4D82-982E-272DECE46C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F917184E-19A6-4E1B-9BA6-6913DBDE1E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{8D2EA155-85C0-46ED-952A-766C040DD7F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8A10AC6D-5D22-40D9-B650-546FBC3E3377}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,29 +36,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+  <si>
+    <t>S. No</t>
+  </si>
+  <si>
+    <t>MRD No</t>
+  </si>
+  <si>
+    <t>Participant ID</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Date of Test</t>
+  </si>
   <si>
     <t>Right Ear</t>
   </si>
   <si>
-    <t>S.No</t>
-  </si>
-  <si>
-    <t>MRD No</t>
-  </si>
-  <si>
-    <t>Patient Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age </t>
-  </si>
-  <si>
-    <t>Gender</t>
+    <t>Right Ear - Pure Tones Average</t>
   </si>
   <si>
     <t>Left Ear</t>
   </si>
   <si>
+    <t>Left Ear - Pure Tones Average</t>
+  </si>
+  <si>
     <t>AC 250</t>
   </si>
   <si>
@@ -77,6 +86,24 @@
     <t>AC 8k</t>
   </si>
   <si>
+    <t>AC 250 (Mask)</t>
+  </si>
+  <si>
+    <t>AC 500 (Mask)</t>
+  </si>
+  <si>
+    <t>AC 1K (Mask)</t>
+  </si>
+  <si>
+    <t>AC 2K (Mask)</t>
+  </si>
+  <si>
+    <t>AC 4K (Mask)</t>
+  </si>
+  <si>
+    <t>AC 8K (Mask)</t>
+  </si>
+  <si>
     <t>BC 250</t>
   </si>
   <si>
@@ -95,53 +122,86 @@
     <t>BC 8k</t>
   </si>
   <si>
-    <t>Participant ID</t>
-  </si>
-  <si>
-    <t>Date</t>
+    <t>BC 250 (Mask)</t>
+  </si>
+  <si>
+    <t>BC 500 (Mask)</t>
+  </si>
+  <si>
+    <t>BC 1K (Mask)</t>
+  </si>
+  <si>
+    <t>BC 2K (Mask)</t>
+  </si>
+  <si>
+    <t>BC 4K (Mask)</t>
+  </si>
+  <si>
+    <t>BC 8K (Mask)</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>BC 1k (Mask)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -149,23 +209,123 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -185,9 +345,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,39 +355,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -279,7 +439,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -331,7 +491,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -390,6 +550,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -398,13 +565,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -469,204 +629,291 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EE587E-75C7-4B62-8D0F-C20F7295F0FC}">
-  <dimension ref="A1:AH3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2617225-28D5-4065-9CC1-A4B21C9A8D4F}">
+  <dimension ref="A1:BF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AD3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="13" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF1" s="10"/>
+    </row>
+    <row r="2" spans="1:58" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="G5" s="4"/>
     </row>
-    <row r="3" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="T1:AE1"/>
+  <mergeCells count="10">
+    <mergeCell ref="G1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:S1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>